<commit_message>
edited the master user stories list, found a typo!
</commit_message>
<xml_diff>
--- a/UserStories_Master.xlsx
+++ b/UserStories_Master.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sojung\SlimPickins\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51985498-D6C7-4485-9F46-7E707736344C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74B7910B-0DA7-400D-B81A-BF5E0BE32869}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11063" windowHeight="9728" xr2:uid="{F1C0E719-113E-4940-B71A-09BA9EE788EC}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="40">
   <si>
     <t>I want to be able to set and track cheat days with SlimPickin</t>
   </si>
@@ -38,9 +38,6 @@
     <t>Description (As a user…)</t>
   </si>
   <si>
-    <t>I want to see my recent history of diet in reverse chronological order when I am viewing the main form/interface</t>
-  </si>
-  <si>
     <t>Comments</t>
   </si>
   <si>
@@ -98,9 +95,6 @@
     <t>I want to be able to delete food from my daily log when I've made an error</t>
   </si>
   <si>
-    <t>I want to be able to view and/or edit food from my daily log when I've made an error</t>
-  </si>
-  <si>
     <t>I want to be able to create a food record and add it to the existing food database</t>
   </si>
   <si>
@@ -137,22 +131,25 @@
     <t>Exercise</t>
   </si>
   <si>
-    <t>I want to be able to navigate to a "favorites" tab from Search to be able to see my recent/favorite foods/meals/snacks/exercises</t>
-  </si>
-  <si>
     <t>I want to be able to just set my diet style (i.e. vegan/paleo/keto) and let SlimPickin generate recommend list of food for me in a "recommendations" tab</t>
   </si>
   <si>
     <t>I want to navigate to a "profile" page that prompts me for my name, email, dietary restrictions/sensitivities/preference and calorie goals per day</t>
   </si>
   <si>
-    <t>When I go to view a food record in the database, I want to see the serving size, calories, dietary restriction (allergies, diabetes, etc), diet preference (vegan, keto, etc)</t>
-  </si>
-  <si>
     <t>I want to be made aware what food is in the season right now in a "In Season" tab from the search page</t>
   </si>
   <si>
     <t>Profile?</t>
+  </si>
+  <si>
+    <t>I want to be able to navigate to a "favorites" tab from Search to be able to see my recent/favorite foods/meals/snacks</t>
+  </si>
+  <si>
+    <t>I want to navigate to the recent history tab in search of diet to see what foods I've added recently</t>
+  </si>
+  <si>
+    <t>When I go to view a food record in the database, I want to see the serving size, calories, dietary restriction (allergies, diabetes, etc), diet preference (vegan, keto, etc), and whether it's a "favorite"</t>
   </si>
 </sst>
 </file>
@@ -241,10 +238,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CC74CACA-FDDF-40D2-AA18-4128115ABBDA}" name="Table1" displayName="Table1" ref="A1:E28" totalsRowShown="0" dataDxfId="5">
-  <autoFilter ref="A1:E28" xr:uid="{84D1842F-7E08-4371-B087-68B771BE479E}"/>
-  <sortState ref="A2:E28">
-    <sortCondition ref="A1:A28"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CC74CACA-FDDF-40D2-AA18-4128115ABBDA}" name="Table1" displayName="Table1" ref="A1:E27" totalsRowShown="0" dataDxfId="5">
+  <autoFilter ref="A1:E27" xr:uid="{84D1842F-7E08-4371-B087-68B771BE479E}"/>
+  <sortState ref="A2:E27">
+    <sortCondition ref="A1:A27"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="4" xr3:uid="{4FEE9258-752C-4ABF-ACAB-254509FF5B0B}" name="Sprint (1-4)" dataDxfId="2"/>
@@ -554,10 +551,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40F826C9-F918-4B64-A9DA-81A4468420CA}">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="103" zoomScaleNormal="103" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="103" zoomScaleNormal="103" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -571,19 +568,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.45">
@@ -591,13 +588,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E2" s="1"/>
     </row>
@@ -606,13 +603,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E3" s="1"/>
     </row>
@@ -621,13 +618,13 @@
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E4" s="1"/>
     </row>
@@ -635,14 +632,14 @@
       <c r="A5" s="2">
         <v>1</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>14</v>
+      <c r="B5" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E5" s="1"/>
     </row>
@@ -650,14 +647,14 @@
       <c r="A6" s="2">
         <v>1</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>14</v>
+      <c r="B6" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E6" s="1"/>
     </row>
@@ -665,14 +662,14 @@
       <c r="A7" s="2">
         <v>1</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>14</v>
+      <c r="B7" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E7" s="1"/>
     </row>
@@ -681,13 +678,13 @@
         <v>1</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E8" s="1"/>
     </row>
@@ -696,36 +693,36 @@
         <v>1</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E9" s="1"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A10" s="2">
+      <c r="A10" s="1">
         <v>1</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>14</v>
+      <c r="B10" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E10" s="1"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A11" s="1">
+      <c r="A11" s="2">
         <v>1</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C11" s="1" t="s">
@@ -741,13 +738,13 @@
         <v>2</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E12" s="1"/>
     </row>
@@ -756,13 +753,13 @@
         <v>2</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E13" s="1"/>
     </row>
@@ -771,13 +768,13 @@
         <v>2</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E14" s="1"/>
     </row>
@@ -786,13 +783,13 @@
         <v>2</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E15" s="1"/>
     </row>
@@ -801,13 +798,13 @@
         <v>2</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E16" s="1"/>
     </row>
@@ -816,13 +813,13 @@
         <v>2</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E17" s="1"/>
     </row>
@@ -831,13 +828,13 @@
         <v>2</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C18" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" s="4" t="s">
         <v>32</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>34</v>
       </c>
       <c r="E18" s="1"/>
     </row>
@@ -846,43 +843,43 @@
         <v>2</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E19" s="1"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A20" s="2">
+      <c r="A20" s="1">
         <v>2</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>15</v>
+      <c r="B20" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>35</v>
+        <v>10</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E20" s="1"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A21" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E21" s="1"/>
     </row>
@@ -891,13 +888,13 @@
         <v>3</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E22" s="1"/>
     </row>
@@ -906,10 +903,10 @@
         <v>3</v>
       </c>
       <c r="B23" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>6</v>
@@ -924,7 +921,7 @@
         <v>14</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>17</v>
+        <v>38</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>7</v>
@@ -939,10 +936,10 @@
         <v>15</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>2</v>
+        <v>33</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E25" s="1"/>
     </row>
@@ -951,13 +948,13 @@
         <v>3</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E26" s="1"/>
     </row>
@@ -966,34 +963,33 @@
         <v>3</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>39</v>
+        <v>0</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="E27" s="1"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A28" s="1">
-        <v>3</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="E28" s="1"/>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="A20:A28 A2:A11">
-    <cfRule type="dataBar" priority="19">
+  <conditionalFormatting sqref="A2:A27">
+    <cfRule type="dataBar" priority="25">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{AD29D292-F5DC-4AB9-8CCB-34B7BF4B1E47}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A20:A27 A2:A11">
+    <cfRule type="dataBar" priority="26">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -1002,20 +998,6 @@
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
           <x14:id>{78473067-DC27-418F-B200-20ED3232141A}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A2:A28">
-    <cfRule type="dataBar" priority="22">
-      <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF638EC6"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{AD29D292-F5DC-4AB9-8CCB-34B7BF4B1E47}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -1029,6 +1011,19 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{AD29D292-F5DC-4AB9-8CCB-34B7BF4B1E47}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>A2:A27</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{78473067-DC27-418F-B200-20ED3232141A}">
             <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
               <x14:cfvo type="autoMin"/>
@@ -1039,20 +1034,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>A20:A28 A2:A11</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{AD29D292-F5DC-4AB9-8CCB-34B7BF4B1E47}">
-            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
-              <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="autoMax"/>
-              <x14:borderColor rgb="FF638EC6"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:negativeBorderColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>A2:A28</xm:sqref>
+          <xm:sqref>A20:A27 A2:A11</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>

<commit_message>
added some comments and changed userstories for which page the stories belong.'
</commit_message>
<xml_diff>
--- a/UserStories_Master.xlsx
+++ b/UserStories_Master.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sojung\SlimPickins\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OneDrive\CS\AD320\Proj1\SlimPickins\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74B7910B-0DA7-400D-B81A-BF5E0BE32869}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="23" documentId="13_ncr:1_{74B7910B-0DA7-400D-B81A-BF5E0BE32869}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{B1985731-A381-47AE-8E13-42F84C37D84C}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11063" windowHeight="9728" xr2:uid="{F1C0E719-113E-4940-B71A-09BA9EE788EC}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11070" windowHeight="9735" xr2:uid="{F1C0E719-113E-4940-B71A-09BA9EE788EC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="43">
   <si>
     <t>I want to be able to set and track cheat days with SlimPickin</t>
   </si>
@@ -140,16 +140,25 @@
     <t>I want to be made aware what food is in the season right now in a "In Season" tab from the search page</t>
   </si>
   <si>
-    <t>Profile?</t>
-  </si>
-  <si>
     <t>I want to be able to navigate to a "favorites" tab from Search to be able to see my recent/favorite foods/meals/snacks</t>
   </si>
   <si>
     <t>I want to navigate to the recent history tab in search of diet to see what foods I've added recently</t>
   </si>
   <si>
-    <t>When I go to view a food record in the database, I want to see the serving size, calories, dietary restriction (allergies, diabetes, etc), diet preference (vegan, keto, etc), and whether it's a "favorite"</t>
+    <t>Search &amp; Info Display</t>
+  </si>
+  <si>
+    <t>Not sure if this means that user is updating his/er own exercise or the general exercise database</t>
+  </si>
+  <si>
+    <t>profile &amp; Info Display</t>
+  </si>
+  <si>
+    <t>When I go to view a food record in the database, I want to see the serving size, calories, dietary restriction (allergies, diabetes, etc), diet preference (vegan, keto, etc.), and whether it's a "favorite"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I was imagine we will have a page for user to go directly to for all his information visualized with additional info displays about lifestyle recommendations and etc. </t>
   </si>
 </sst>
 </file>
@@ -212,13 +221,13 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -240,15 +249,15 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CC74CACA-FDDF-40D2-AA18-4128115ABBDA}" name="Table1" displayName="Table1" ref="A1:E27" totalsRowShown="0" dataDxfId="5">
   <autoFilter ref="A1:E27" xr:uid="{84D1842F-7E08-4371-B087-68B771BE479E}"/>
-  <sortState ref="A2:E27">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E27">
     <sortCondition ref="A1:A27"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="4" xr3:uid="{4FEE9258-752C-4ABF-ACAB-254509FF5B0B}" name="Sprint (1-4)" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{50BA2B0E-C671-41C9-8CBF-24048D0570F7}" name="User Level" dataDxfId="0"/>
-    <tableColumn id="2" xr3:uid="{FD85E7F2-8C77-40F5-8F0A-6774FC0B0C93}" name="Description (As a user…)" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{4FEE9258-752C-4ABF-ACAB-254509FF5B0B}" name="Sprint (1-4)" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{50BA2B0E-C671-41C9-8CBF-24048D0570F7}" name="User Level" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{FD85E7F2-8C77-40F5-8F0A-6774FC0B0C93}" name="Description (As a user…)" dataDxfId="2"/>
     <tableColumn id="5" xr3:uid="{72D361D2-3237-4B06-8B73-B209CEB6A8AF}" name="Page" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{ABDB9176-0088-43CB-A3DF-E8418D2E8E38}" name="Comments" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{ABDB9176-0088-43CB-A3DF-E8418D2E8E38}" name="Comments" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -554,19 +563,19 @@
   <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="103" zoomScaleNormal="103" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="12.19921875" customWidth="1"/>
-    <col min="3" max="3" width="125.3984375" customWidth="1"/>
-    <col min="4" max="4" width="14.06640625" customWidth="1"/>
-    <col min="5" max="5" width="22.6640625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="19.06640625" customWidth="1"/>
+    <col min="1" max="2" width="12.140625" customWidth="1"/>
+    <col min="3" max="3" width="194.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" customWidth="1"/>
+    <col min="5" max="5" width="22.7109375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -583,7 +592,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -598,7 +607,7 @@
       </c>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -609,11 +618,11 @@
         <v>19</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -628,7 +637,7 @@
       </c>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>1</v>
       </c>
@@ -636,14 +645,14 @@
         <v>13</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>1</v>
       </c>
@@ -658,7 +667,7 @@
       </c>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>1</v>
       </c>
@@ -673,7 +682,7 @@
       </c>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>1</v>
       </c>
@@ -688,7 +697,7 @@
       </c>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>1</v>
       </c>
@@ -703,7 +712,7 @@
       </c>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>1</v>
       </c>
@@ -718,7 +727,7 @@
       </c>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>1</v>
       </c>
@@ -726,14 +735,14 @@
         <v>14</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>2</v>
       </c>
@@ -744,11 +753,11 @@
         <v>24</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>2</v>
       </c>
@@ -763,7 +772,7 @@
       </c>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>2</v>
       </c>
@@ -778,7 +787,7 @@
       </c>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>2</v>
       </c>
@@ -789,11 +798,11 @@
         <v>27</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>2</v>
       </c>
@@ -804,11 +813,11 @@
         <v>28</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>2</v>
       </c>
@@ -819,11 +828,11 @@
         <v>29</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>2</v>
       </c>
@@ -838,7 +847,7 @@
       </c>
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>2</v>
       </c>
@@ -851,9 +860,11 @@
       <c r="D19" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="E19" s="1"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="E19" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>2</v>
       </c>
@@ -868,7 +879,7 @@
       </c>
       <c r="E20" s="1"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>3</v>
       </c>
@@ -883,7 +894,7 @@
       </c>
       <c r="E21" s="1"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>3</v>
       </c>
@@ -898,7 +909,7 @@
       </c>
       <c r="E22" s="1"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>3</v>
       </c>
@@ -913,7 +924,7 @@
       </c>
       <c r="E23" s="1"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>3</v>
       </c>
@@ -921,14 +932,14 @@
         <v>14</v>
       </c>
       <c r="C24" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D24" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D24" s="4" t="s">
-        <v>7</v>
-      </c>
       <c r="E24" s="1"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>3</v>
       </c>
@@ -939,11 +950,13 @@
         <v>33</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E25" s="1"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
+        <v>40</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>3</v>
       </c>
@@ -954,11 +967,11 @@
         <v>35</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="E26" s="1"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>3</v>
       </c>
@@ -969,7 +982,7 @@
         <v>0</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="E27" s="1"/>
     </row>

</xml_diff>